<commit_message>
refactor: rewrite encoder (#5)
</commit_message>
<xml_diff>
--- a/encoding/xlsform/testdata/group.xlsx
+++ b/encoding/xlsform/testdata/group.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">label:English</t>
+    <t xml:space="preserve">label::English (en)</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label::English (en)</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -199,10 +196,10 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -308,7 +305,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -329,7 +326,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -340,30 +337,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>